<commit_message>
wax dipping st curve and data
</commit_message>
<xml_diff>
--- a/Dec-July-2019-analysis/data/Physiology-URI-labwork.xlsx
+++ b/Dec-July-2019-analysis/data/Physiology-URI-labwork.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/Dec-July-2019-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA503CA-1F5C-9940-8FE6-445EC010EA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF38F181-021D-DD4E-827F-0654EC106B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="460" windowWidth="27820" windowHeight="19560" activeTab="1" xr2:uid="{A8334511-D0E0-DA42-8F89-A6B529CE2D9F}"/>
+    <workbookView xWindow="5780" yWindow="460" windowWidth="27820" windowHeight="19560" xr2:uid="{A8334511-D0E0-DA42-8F89-A6B529CE2D9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
-    <sheet name="Counts" sheetId="4" r:id="rId2"/>
-    <sheet name="Chlorophyll platemap for .csv" sheetId="3" r:id="rId3"/>
-    <sheet name="Chlorophyll 96 well platemap" sheetId="5" r:id="rId4"/>
+    <sheet name="Surface_area" sheetId="6" r:id="rId2"/>
+    <sheet name="Counts" sheetId="4" r:id="rId3"/>
+    <sheet name="Chlorophyll platemap for .csv" sheetId="3" r:id="rId4"/>
+    <sheet name="Chlorophyll 96 well platemap" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="199">
   <si>
     <t>ColonyID</t>
   </si>
@@ -625,6 +626,15 @@
   </si>
   <si>
     <t>don't have this fragment</t>
+  </si>
+  <si>
+    <t>Weight1</t>
+  </si>
+  <si>
+    <t>Weight2</t>
+  </si>
+  <si>
+    <t>WaxID</t>
   </si>
 </sst>
 </file>
@@ -715,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -729,6 +739,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,8 +1070,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2208,14 +2219,708 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D07E79-F9DC-3749-8FFA-555D86B705D8}">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.1686</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.46710000000000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.47239999999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.54110000000000003</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.51490000000000002</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.58530000000000004</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>201</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>202</v>
+      </c>
+      <c r="B9" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.4304</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.50380000000000003</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>203</v>
+      </c>
+      <c r="B10" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>204</v>
+      </c>
+      <c r="B11" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.1789</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.219</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>209</v>
+      </c>
+      <c r="B12" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>210</v>
+      </c>
+      <c r="B13" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.3402</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.39290000000000003</v>
+      </c>
+      <c r="E13" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>211</v>
+      </c>
+      <c r="B14" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.6400000000000001E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>212</v>
+      </c>
+      <c r="B15" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.2198</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.25290000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>217</v>
+      </c>
+      <c r="B16" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.2442</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>218</v>
+      </c>
+      <c r="B17" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.31259999999999999</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.3634</v>
+      </c>
+      <c r="E17" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>219</v>
+      </c>
+      <c r="B18" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.8095</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>220</v>
+      </c>
+      <c r="B19" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.0266</v>
+      </c>
+      <c r="E19" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>221</v>
+      </c>
+      <c r="B20" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.25569999999999998</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.31119999999999998</v>
+      </c>
+      <c r="E20" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>222</v>
+      </c>
+      <c r="B21" s="4">
+        <v>43662</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.1215</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.1721</v>
+      </c>
+      <c r="E21" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.20050000000000001</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.24779999999999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.1671999999999998</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2.4702000000000002</v>
+      </c>
+      <c r="E23" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>11</v>
+      </c>
+      <c r="B24" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.32729999999999998</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.4037</v>
+      </c>
+      <c r="E24" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>12</v>
+      </c>
+      <c r="B25" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.2319</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.26910000000000001</v>
+      </c>
+      <c r="E25" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.9127999999999998</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.2977999999999996</v>
+      </c>
+      <c r="E26" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2.7490000000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.1577999999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>201</v>
+      </c>
+      <c r="B28" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.0439000000000001</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.1748000000000001</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>202</v>
+      </c>
+      <c r="B29" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.82630000000000003</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.93730000000000002</v>
+      </c>
+      <c r="E29" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>203</v>
+      </c>
+      <c r="B30" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.7258</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="E30" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>204</v>
+      </c>
+      <c r="B31" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1.0881000000000001</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1.2442</v>
+      </c>
+      <c r="E31" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>209</v>
+      </c>
+      <c r="B32" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.34920000000000001</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.42620000000000002</v>
+      </c>
+      <c r="E32" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>210</v>
+      </c>
+      <c r="B33" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.12230000000000001</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.16320000000000001</v>
+      </c>
+      <c r="E33" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>211</v>
+      </c>
+      <c r="B34" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.6887000000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.9319</v>
+      </c>
+      <c r="E34" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>212</v>
+      </c>
+      <c r="B35" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.34510000000000002</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.41909999999999997</v>
+      </c>
+      <c r="E35" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>217</v>
+      </c>
+      <c r="B36" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.56930000000000003</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.6804</v>
+      </c>
+      <c r="E36" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>218</v>
+      </c>
+      <c r="B37" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1.5530999999999999</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1.7079</v>
+      </c>
+      <c r="E37" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>219</v>
+      </c>
+      <c r="B38" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1.0459000000000001</v>
+      </c>
+      <c r="E38" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>220</v>
+      </c>
+      <c r="B39" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="E39" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>221</v>
+      </c>
+      <c r="B40" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.1215</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.1721</v>
+      </c>
+      <c r="E40" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>222</v>
+      </c>
+      <c r="B41" s="4">
+        <v>43803</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.3095</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.38109999999999999</v>
+      </c>
+      <c r="E41" s="2">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EF6ABA-4D29-C044-9AC4-5E3D52622500}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3851,7 +4556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA606780-F822-BD46-A838-06BD626AFE1E}">
   <dimension ref="A1:C97"/>
   <sheetViews>
@@ -4934,7 +5639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7DFA2A-7D1C-274C-8D36-2EDA7274E323}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>